<commit_message>
Set up hubway experiments
</commit_message>
<xml_diff>
--- a/Experiments/Experiment_1/results/aggregate_results_experiment1.xlsx
+++ b/Experiments/Experiment_1/results/aggregate_results_experiment1.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="13200" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$N$57</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$N$68</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="28">
   <si>
     <t>seed</t>
   </si>
@@ -109,12 +109,22 @@
   <si>
     <t>newdunn (min10)</t>
   </si>
+  <si>
+    <t>newdunn (min25)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -131,12 +141,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -148,15 +164,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="11" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -432,18 +451,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N57"/>
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A1:T68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="M33" sqref="A26:M33"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="106" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
+    <col min="5" max="10" width="0" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -487,408 +510,412 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>2</v>
-      </c>
-      <c r="B2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2">
         <v>6</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>8</v>
       </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2">
+      <c r="D2" s="2">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2">
         <v>0.49210636592436302</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="2">
         <v>0.60000550341052605</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="2">
         <v>0.562048331967263</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="2">
         <v>0.31132505700394297</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="2">
         <v>0.79275920098328401</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="2">
         <v>0.188533603208666</v>
       </c>
-      <c r="K2">
-        <v>-10</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="K2" s="2">
+        <v>-10</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>4</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2">
+        <v>4</v>
+      </c>
+      <c r="D3" s="2">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2">
         <v>0.368742013243754</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="2">
         <v>0.48287658388833898</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="2">
         <v>0.416629377645171</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="2">
         <v>0.31132505700394297</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="2">
         <v>0.23008166516200601</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="2">
         <v>0.188533603208666</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="2">
         <v>0.123619262971653</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N3" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>4</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2">
+        <v>4</v>
+      </c>
+      <c r="D4" s="2">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2">
         <v>0.13687273124836999</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="2">
         <v>2.9254822561079901E-2</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="2">
         <v>2.29642246628344E-2</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="2">
         <v>0.371070999354494</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="2">
         <v>-3.5810028561957898E-3</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="2">
         <v>0.188533603208666</v>
       </c>
-      <c r="K4" s="1">
+      <c r="K4" s="3">
         <v>1.2515800807311799E-5</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5">
+      <c r="P4" s="2"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2">
+        <v>2</v>
+      </c>
+      <c r="E5" s="2">
         <v>8.50766061483436E-2</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="2">
         <v>2.9254822561079901E-2</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="2">
         <v>2.29642246628344E-2</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="2">
         <v>0.371070999354494</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="2">
         <v>2.5811887429712601E-2</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="2">
         <v>0.188533603208666</v>
       </c>
-      <c r="K5" s="1">
+      <c r="K5" s="3">
         <v>7.5095737678586007E-5</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="N5" t="s">
+      <c r="N5" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6">
-        <v>4</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6">
+    <row r="6" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2">
+        <v>4</v>
+      </c>
+      <c r="D6" s="2">
+        <v>2</v>
+      </c>
+      <c r="E6" s="2">
         <v>0.226113806232564</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="2">
         <v>0.49802205880935102</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="2">
         <v>0.40386509685451399</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="2">
         <v>0.43557908247046601</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="2">
         <v>-3.5810028561957898E-3</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="2">
         <v>0.188533603208666</v>
       </c>
-      <c r="K6" s="1">
+      <c r="K6" s="3">
         <v>1.2515800807311799E-5</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="N6" t="s">
+      <c r="N6" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7">
-        <v>4</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="E7">
+    <row r="7" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2">
+        <v>2</v>
+      </c>
+      <c r="C7" s="2">
+        <v>4</v>
+      </c>
+      <c r="D7" s="2">
+        <v>2</v>
+      </c>
+      <c r="E7" s="2">
         <v>0.226113806232564</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="2">
         <v>0.49802205880935102</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="2">
         <v>0.40386509685451399</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="2">
         <v>0.43557908247046601</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="2">
         <v>-3.5810028561957898E-3</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="2">
         <v>0.188533603208666</v>
       </c>
-      <c r="K7" s="1">
+      <c r="K7" s="3">
         <v>1.2515800807311799E-5</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="N7" t="s">
+      <c r="N7" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>2</v>
-      </c>
-      <c r="B8">
+    <row r="8" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>2</v>
+      </c>
+      <c r="B8" s="2">
         <v>6</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>8</v>
       </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
-      <c r="E8">
+      <c r="D8" s="2">
+        <v>2</v>
+      </c>
+      <c r="E8" s="2">
         <v>0.33191092053589</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="2">
         <v>0.63534817479215899</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="2">
         <v>0.540898005765868</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="2">
         <v>0.43557908247046601</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="2">
         <v>0.40176654302611697</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="2">
         <v>0.188533603208666</v>
       </c>
-      <c r="K8">
-        <v>-10</v>
-      </c>
-      <c r="L8" t="s">
+      <c r="K8" s="2">
+        <v>-10</v>
+      </c>
+      <c r="L8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N8" t="s">
+      <c r="N8" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>2</v>
-      </c>
-      <c r="B9">
+    <row r="9" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>2</v>
+      </c>
+      <c r="B9" s="2">
         <v>8</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="2">
         <v>10</v>
       </c>
-      <c r="D9">
-        <v>2</v>
-      </c>
-      <c r="E9">
+      <c r="D9" s="2">
+        <v>2</v>
+      </c>
+      <c r="E9" s="2">
         <v>0.31900944422074201</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="2">
         <v>0.68792922961345104</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="2">
         <v>0.63534817479215899</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="2">
         <v>0.43557908247046601</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="2">
         <v>0.45517720518341698</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="2">
         <v>0.188533603208666</v>
       </c>
-      <c r="K9">
-        <v>-10</v>
-      </c>
-      <c r="L9" t="s">
+      <c r="K9" s="2">
+        <v>-10</v>
+      </c>
+      <c r="L9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="M9" t="s">
+      <c r="M9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N9" t="s">
+      <c r="N9" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>2</v>
-      </c>
-      <c r="B10">
-        <v>4</v>
-      </c>
-      <c r="C10">
-        <v>7</v>
-      </c>
-      <c r="D10">
-        <v>7</v>
-      </c>
-      <c r="E10">
-        <v>0.45507180711967898</v>
-      </c>
-      <c r="F10">
-        <v>0.70170122087426401</v>
-      </c>
-      <c r="G10">
-        <v>0.429659018054111</v>
-      </c>
-      <c r="H10">
-        <v>0.70170122087426401</v>
-      </c>
-      <c r="I10">
-        <v>0.308058712082381</v>
-      </c>
-      <c r="J10">
-        <v>1</v>
-      </c>
-      <c r="K10">
-        <v>-10</v>
-      </c>
-      <c r="L10" t="s">
-        <v>19</v>
-      </c>
-      <c r="M10" t="s">
-        <v>15</v>
-      </c>
-      <c r="N10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>2</v>
+      </c>
+      <c r="B10" s="2">
+        <v>4</v>
+      </c>
+      <c r="C10" s="2">
+        <v>6</v>
+      </c>
+      <c r="D10" s="2">
+        <v>2</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.44193928617146799</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.540898005765868</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0.49802205880935102</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0.43557908247046601</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0.375576819861136</v>
+      </c>
+      <c r="J10" s="2">
+        <v>0.188533603208666</v>
+      </c>
+      <c r="K10" s="2">
+        <v>-10</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C11">
         <v>7</v>
@@ -897,19 +924,19 @@
         <v>7</v>
       </c>
       <c r="E11">
-        <v>0.28143846997518301</v>
+        <v>0.45507180711967898</v>
       </c>
       <c r="F11">
         <v>0.70170122087426401</v>
       </c>
       <c r="G11">
-        <v>0.35696399001995099</v>
+        <v>0.429659018054111</v>
       </c>
       <c r="H11">
         <v>0.70170122087426401</v>
       </c>
       <c r="I11">
-        <v>0.27042566468741702</v>
+        <v>0.308058712082381</v>
       </c>
       <c r="J11">
         <v>1</v>
@@ -924,15 +951,15 @@
         <v>15</v>
       </c>
       <c r="N11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2</v>
       </c>
       <c r="B12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C12">
         <v>7</v>
@@ -941,19 +968,19 @@
         <v>7</v>
       </c>
       <c r="E12">
-        <v>0.35747522343877502</v>
+        <v>0.28143846997518301</v>
       </c>
       <c r="F12">
-        <v>1.0761834076521399</v>
+        <v>0.70170122087426401</v>
       </c>
       <c r="G12">
-        <v>0.104346361683884</v>
+        <v>0.35696399001995099</v>
       </c>
       <c r="H12">
-        <v>1.0761834076521399</v>
+        <v>0.70170122087426401</v>
       </c>
       <c r="I12">
-        <v>0.44241624371686999</v>
+        <v>0.27042566468741702</v>
       </c>
       <c r="J12">
         <v>1</v>
@@ -965,18 +992,18 @@
         <v>19</v>
       </c>
       <c r="M12" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="N12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C13">
         <v>7</v>
@@ -985,19 +1012,19 @@
         <v>7</v>
       </c>
       <c r="E13">
-        <v>0.30026895854105601</v>
+        <v>0.35747522343877502</v>
       </c>
       <c r="F13">
         <v>1.0761834076521399</v>
       </c>
       <c r="G13">
-        <v>2.8271345480450499E-2</v>
+        <v>0.104346361683884</v>
       </c>
       <c r="H13">
         <v>1.0761834076521399</v>
       </c>
       <c r="I13">
-        <v>-6.6932199712796403E-2</v>
+        <v>0.44241624371686999</v>
       </c>
       <c r="J13">
         <v>1</v>
@@ -1012,15 +1039,15 @@
         <v>18</v>
       </c>
       <c r="N13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2</v>
       </c>
       <c r="B14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C14">
         <v>7</v>
@@ -1029,19 +1056,19 @@
         <v>7</v>
       </c>
       <c r="E14">
-        <v>0.44130793008930003</v>
+        <v>0.30026895854105601</v>
       </c>
       <c r="F14">
-        <v>1.2743172301085499</v>
+        <v>1.0761834076521399</v>
       </c>
       <c r="G14">
-        <v>0.35651092069156698</v>
+        <v>2.8271345480450499E-2</v>
       </c>
       <c r="H14">
-        <v>1.2743172301085499</v>
+        <v>1.0761834076521399</v>
       </c>
       <c r="I14">
-        <v>0.21459260311925801</v>
+        <v>-6.6932199712796403E-2</v>
       </c>
       <c r="J14">
         <v>1</v>
@@ -1053,13 +1080,13 @@
         <v>19</v>
       </c>
       <c r="M14" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="N14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1100,10 +1127,10 @@
         <v>25</v>
       </c>
       <c r="N15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2</v>
       </c>
@@ -1137,17 +1164,17 @@
       <c r="K16">
         <v>-10</v>
       </c>
-      <c r="L16" s="2" t="s">
+      <c r="L16" t="s">
         <v>19</v>
       </c>
       <c r="M16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1181,17 +1208,17 @@
       <c r="K17">
         <v>-10</v>
       </c>
-      <c r="L17" t="s">
+      <c r="L17" s="1" t="s">
         <v>19</v>
       </c>
       <c r="M17" t="s">
         <v>26</v>
       </c>
       <c r="N17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2</v>
       </c>
@@ -1199,125 +1226,125 @@
         <v>4</v>
       </c>
       <c r="C18">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D18">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E18">
-        <v>0.56630547456343205</v>
+        <v>0.44130793008930003</v>
       </c>
       <c r="F18">
-        <v>0.56775605437586296</v>
+        <v>1.2743172301085499</v>
       </c>
       <c r="G18">
-        <v>0.56775605437586296</v>
+        <v>0.35651092069156698</v>
       </c>
       <c r="H18">
-        <v>0.43936196984910503</v>
+        <v>1.2743172301085499</v>
       </c>
       <c r="I18">
-        <v>0.96551156243106095</v>
+        <v>0.21459260311925801</v>
       </c>
       <c r="J18">
-        <v>0.42156123687451802</v>
+        <v>1</v>
       </c>
       <c r="K18">
         <v>-10</v>
       </c>
       <c r="L18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M18" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="N18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C19">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D19">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E19">
-        <v>0.405800430501631</v>
+        <v>0.44737814540257398</v>
       </c>
       <c r="F19">
-        <v>0.56775605437586296</v>
+        <v>1.2743172301085499</v>
       </c>
       <c r="G19">
-        <v>0.40504950735346601</v>
+        <v>0.35651092069156698</v>
       </c>
       <c r="H19">
-        <v>0.43936196984910503</v>
+        <v>1.2743172301085499</v>
       </c>
       <c r="I19">
-        <v>2.0028615322726501E-2</v>
+        <v>0.71113130698584803</v>
       </c>
       <c r="J19">
-        <v>0.42156123687451802</v>
+        <v>1</v>
       </c>
       <c r="K19">
         <v>-10</v>
       </c>
       <c r="L19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M19" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="N19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2</v>
       </c>
       <c r="B20">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C20">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D20">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E20">
-        <v>0.117052395539751</v>
+        <v>0.44737814540257398</v>
       </c>
       <c r="F20">
-        <v>3.53340640999271E-2</v>
+        <v>1.2743172301085499</v>
       </c>
       <c r="G20">
-        <v>3.53340640999271E-2</v>
+        <v>0.35651092069156698</v>
       </c>
       <c r="H20">
-        <v>0.117052395539751</v>
+        <v>1.2743172301085499</v>
       </c>
       <c r="I20">
-        <v>0.42156123687451802</v>
+        <v>0.71113130698584803</v>
       </c>
       <c r="J20">
-        <v>0.42156123687451802</v>
+        <v>1</v>
       </c>
       <c r="K20">
-        <v>1</v>
+        <v>-10</v>
       </c>
       <c r="L20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M20" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="N20" t="s">
         <v>16</v>
@@ -1328,28 +1355,28 @@
         <v>2</v>
       </c>
       <c r="B21">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D21">
         <v>3</v>
       </c>
       <c r="E21">
-        <v>8.4695981752626395E-2</v>
+        <v>0.56630547456343205</v>
       </c>
       <c r="F21">
-        <v>3.53340640999271E-2</v>
+        <v>0.56775605437586296</v>
       </c>
       <c r="G21">
-        <v>2.9519585670639299E-2</v>
+        <v>0.56775605437586296</v>
       </c>
       <c r="H21">
-        <v>0.117052395539751</v>
+        <v>0.43936196984910503</v>
       </c>
       <c r="I21">
-        <v>9.8895515526911605E-4</v>
+        <v>0.96551156243106095</v>
       </c>
       <c r="J21">
         <v>0.42156123687451802</v>
@@ -1361,10 +1388,10 @@
         <v>20</v>
       </c>
       <c r="M21" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="N21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
@@ -1372,28 +1399,28 @@
         <v>2</v>
       </c>
       <c r="B22">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C22">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D22">
         <v>3</v>
       </c>
       <c r="E22">
-        <v>0.24657962351437601</v>
+        <v>0.405800430501631</v>
       </c>
       <c r="F22">
-        <v>0.41820399324290503</v>
+        <v>0.56775605437586296</v>
       </c>
       <c r="G22">
-        <v>0.40832796896392198</v>
+        <v>0.40504950735346601</v>
       </c>
       <c r="H22">
-        <v>0.26423634114378802</v>
+        <v>0.43936196984910503</v>
       </c>
       <c r="I22">
-        <v>0.61588260194142797</v>
+        <v>2.0028615322726501E-2</v>
       </c>
       <c r="J22">
         <v>0.42156123687451802</v>
@@ -1405,7 +1432,7 @@
         <v>20</v>
       </c>
       <c r="M22" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="N22" t="s">
         <v>17</v>
@@ -1416,40 +1443,40 @@
         <v>2</v>
       </c>
       <c r="B23">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C23">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D23">
         <v>3</v>
       </c>
       <c r="E23">
-        <v>0.24657962351437601</v>
+        <v>0.117052395539751</v>
       </c>
       <c r="F23">
-        <v>0.41820399324290503</v>
+        <v>3.53340640999271E-2</v>
       </c>
       <c r="G23">
-        <v>0.40832796896392198</v>
+        <v>3.53340640999271E-2</v>
       </c>
       <c r="H23">
-        <v>0.26423634114378802</v>
+        <v>0.117052395539751</v>
       </c>
       <c r="I23">
-        <v>0.61588260194142797</v>
+        <v>0.42156123687451802</v>
       </c>
       <c r="J23">
         <v>0.42156123687451802</v>
       </c>
       <c r="K23">
-        <v>-10</v>
+        <v>1</v>
       </c>
       <c r="L23" t="s">
         <v>20</v>
       </c>
       <c r="M23" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="N23" t="s">
         <v>16</v>
@@ -1460,28 +1487,28 @@
         <v>2</v>
       </c>
       <c r="B24">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C24">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D24">
         <v>3</v>
       </c>
       <c r="E24">
-        <v>0.24657962351437601</v>
+        <v>8.4695981752626395E-2</v>
       </c>
       <c r="F24">
-        <v>0.41820399324290503</v>
+        <v>3.53340640999271E-2</v>
       </c>
       <c r="G24">
-        <v>0.40832796896392198</v>
+        <v>2.9519585670639299E-2</v>
       </c>
       <c r="H24">
-        <v>0.26423634114378802</v>
+        <v>0.117052395539751</v>
       </c>
       <c r="I24">
-        <v>0.61588260194142797</v>
+        <v>9.8895515526911605E-4</v>
       </c>
       <c r="J24">
         <v>0.42156123687451802</v>
@@ -1493,13 +1520,13 @@
         <v>20</v>
       </c>
       <c r="M24" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="N24" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2</v>
       </c>
@@ -1537,189 +1564,189 @@
         <v>20</v>
       </c>
       <c r="M25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N25" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2</v>
       </c>
       <c r="B26">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C26">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D26">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E26">
-        <v>0.62932589385541504</v>
+        <v>0.24657962351437601</v>
       </c>
       <c r="F26">
-        <v>0.58650943274169698</v>
+        <v>0.41820399324290503</v>
       </c>
       <c r="G26">
-        <v>0.421332397868108</v>
+        <v>0.40832796896392198</v>
       </c>
       <c r="H26">
-        <v>0.29520828013791001</v>
+        <v>0.26423634114378802</v>
       </c>
       <c r="I26">
-        <v>-1.11161715145589E-2</v>
+        <v>0.61588260194142797</v>
       </c>
       <c r="J26">
-        <v>0.63488804766750195</v>
+        <v>0.42156123687451802</v>
       </c>
       <c r="K26">
         <v>-10</v>
       </c>
       <c r="L26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M26" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="N26" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2</v>
       </c>
       <c r="B27">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C27">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D27">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E27">
-        <v>0.62891229169528395</v>
+        <v>0.24657962351437601</v>
       </c>
       <c r="F27">
-        <v>0.58650943274169698</v>
+        <v>0.41820399324290503</v>
       </c>
       <c r="G27">
-        <v>0.421332397868108</v>
+        <v>0.40832796896392198</v>
       </c>
       <c r="H27">
-        <v>0.29520828013791001</v>
+        <v>0.26423634114378802</v>
       </c>
       <c r="I27">
-        <v>1.5749039138464899E-2</v>
+        <v>0.61588260194142797</v>
       </c>
       <c r="J27">
-        <v>0.63488804766750195</v>
+        <v>0.42156123687451802</v>
       </c>
       <c r="K27">
         <v>-10</v>
       </c>
       <c r="L27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M27" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="N27" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2</v>
       </c>
       <c r="B28">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C28">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D28">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E28">
-        <v>0.36170411713162098</v>
+        <v>0.24657962351437601</v>
       </c>
       <c r="F28">
-        <v>2.4674359903005798E-2</v>
+        <v>0.41820399324290503</v>
       </c>
       <c r="G28">
-        <v>1.0986722252429099E-2</v>
+        <v>0.40832796896392198</v>
       </c>
       <c r="H28">
-        <v>0.25329913298274598</v>
+        <v>0.26423634114378802</v>
       </c>
       <c r="I28">
-        <v>-1.11161715145589E-2</v>
+        <v>0.61588260194142797</v>
       </c>
       <c r="J28">
-        <v>0.63488804766750195</v>
+        <v>0.42156123687451802</v>
       </c>
       <c r="K28">
         <v>-10</v>
       </c>
       <c r="L28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M28" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="N28" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2</v>
       </c>
       <c r="B29">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C29">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D29">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E29">
-        <v>0.36166668347144698</v>
+        <v>0.26792111416827502</v>
       </c>
       <c r="F29">
-        <v>2.4674359903005798E-2</v>
+        <v>0.41820399324290503</v>
       </c>
       <c r="G29">
-        <v>1.0986722252429099E-2</v>
+        <v>0.33608886474093502</v>
       </c>
       <c r="H29">
-        <v>0.25329913298274598</v>
+        <v>0.26423634114378802</v>
       </c>
       <c r="I29">
-        <v>1.5749039138464899E-2</v>
+        <v>0.46266029517068802</v>
       </c>
       <c r="J29">
-        <v>0.63488804766750195</v>
+        <v>0.42156123687451802</v>
       </c>
       <c r="K29">
-        <v>-10</v>
+        <v>0.90011182843377002</v>
       </c>
       <c r="L29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M29" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="N29" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2</v>
       </c>
@@ -1727,40 +1754,40 @@
         <v>5</v>
       </c>
       <c r="C30">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D30">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E30">
-        <v>0.65688384913490006</v>
+        <v>0.42210485726329899</v>
       </c>
       <c r="F30">
-        <v>0.56162508846695203</v>
+        <v>0.41820399324290503</v>
       </c>
       <c r="G30">
-        <v>0.40593673391254598</v>
+        <v>0.41820399324290503</v>
       </c>
       <c r="H30">
-        <v>0.30993475094059397</v>
+        <v>0.26423634114378802</v>
       </c>
       <c r="I30">
-        <v>1.87695196954741E-2</v>
+        <v>0.97886397901002997</v>
       </c>
       <c r="J30">
-        <v>0.63488804766750195</v>
+        <v>0.42156123687451802</v>
       </c>
       <c r="K30">
         <v>-10</v>
       </c>
       <c r="L30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M30" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="N30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
@@ -1768,7 +1795,7 @@
         <v>2</v>
       </c>
       <c r="B31">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C31">
         <v>8</v>
@@ -1777,19 +1804,19 @@
         <v>6</v>
       </c>
       <c r="E31">
-        <v>0.65688384913490006</v>
+        <v>0.62932589385541504</v>
       </c>
       <c r="F31">
-        <v>0.56162508846695203</v>
+        <v>0.58650943274169698</v>
       </c>
       <c r="G31">
-        <v>0.40593673391254598</v>
+        <v>0.421332397868108</v>
       </c>
       <c r="H31">
-        <v>0.30993475094059397</v>
+        <v>0.29520828013791001</v>
       </c>
       <c r="I31">
-        <v>1.87695196954741E-2</v>
+        <v>-1.11161715145589E-2</v>
       </c>
       <c r="J31">
         <v>0.63488804766750195</v>
@@ -1801,7 +1828,7 @@
         <v>21</v>
       </c>
       <c r="M31" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="N31" t="s">
         <v>16</v>
@@ -1812,7 +1839,7 @@
         <v>2</v>
       </c>
       <c r="B32">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C32">
         <v>8</v>
@@ -1821,31 +1848,31 @@
         <v>6</v>
       </c>
       <c r="E32">
-        <v>0.27857501901371701</v>
+        <v>0.62891229169528395</v>
       </c>
       <c r="F32">
-        <v>0.56162508846695203</v>
+        <v>0.58650943274169698</v>
       </c>
       <c r="G32">
-        <v>0.42216469549779001</v>
+        <v>0.421332397868108</v>
       </c>
       <c r="H32">
-        <v>0.30993475094059397</v>
+        <v>0.29520828013791001</v>
       </c>
       <c r="I32">
-        <v>0.50057518439717696</v>
+        <v>1.5749039138464899E-2</v>
       </c>
       <c r="J32">
         <v>0.63488804766750195</v>
       </c>
       <c r="K32">
-        <v>0.28031055955788298</v>
+        <v>-10</v>
       </c>
       <c r="L32" t="s">
         <v>21</v>
       </c>
       <c r="M32" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="N32" t="s">
         <v>17</v>
@@ -1856,28 +1883,28 @@
         <v>2</v>
       </c>
       <c r="B33">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C33">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D33">
         <v>6</v>
       </c>
       <c r="E33">
-        <v>0.31685573999791999</v>
+        <v>0.36170411713162098</v>
       </c>
       <c r="F33">
-        <v>0.58470463432173803</v>
+        <v>2.4674359903005798E-2</v>
       </c>
       <c r="G33">
-        <v>0.56162508846695203</v>
+        <v>1.0986722252429099E-2</v>
       </c>
       <c r="H33">
-        <v>0.30993475094059397</v>
+        <v>0.25329913298274598</v>
       </c>
       <c r="I33">
-        <v>0.76576267194731096</v>
+        <v>-1.11161715145589E-2</v>
       </c>
       <c r="J33">
         <v>0.63488804766750195</v>
@@ -1889,7 +1916,7 @@
         <v>21</v>
       </c>
       <c r="M33" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="N33" t="s">
         <v>16</v>
@@ -1900,263 +1927,263 @@
         <v>2</v>
       </c>
       <c r="B34">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C34">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D34">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E34">
-        <v>0.49883257996769198</v>
+        <v>0.36166668347144698</v>
       </c>
       <c r="F34">
-        <v>0.50354162084910403</v>
+        <v>2.4674359903005798E-2</v>
       </c>
       <c r="G34">
-        <v>0.50354162084910403</v>
+        <v>1.0986722252429099E-2</v>
       </c>
       <c r="H34">
-        <v>0.50354162084910403</v>
+        <v>0.25329913298274598</v>
       </c>
       <c r="I34">
-        <v>0.98008594436669005</v>
+        <v>1.5749039138464899E-2</v>
       </c>
       <c r="J34">
-        <v>1</v>
+        <v>0.63488804766750195</v>
       </c>
       <c r="K34">
-        <v>0.98008594436669005</v>
+        <v>-10</v>
       </c>
       <c r="L34" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M34" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="N34" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>2</v>
       </c>
       <c r="B35">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C35">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D35">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E35">
-        <v>0.29309016613321198</v>
+        <v>0.65688384913490006</v>
       </c>
       <c r="F35">
-        <v>0.50354162084910403</v>
+        <v>0.56162508846695203</v>
       </c>
       <c r="G35">
-        <v>0.28473904387460602</v>
+        <v>0.40593673391254598</v>
       </c>
       <c r="H35">
-        <v>0.50354162084910403</v>
+        <v>0.30993475094059397</v>
       </c>
       <c r="I35">
-        <v>0.17879836972409099</v>
+        <v>1.87695196954741E-2</v>
       </c>
       <c r="J35">
-        <v>1</v>
+        <v>0.63488804766750195</v>
       </c>
       <c r="K35">
         <v>-10</v>
       </c>
       <c r="L35" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M35" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="N35" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>2</v>
       </c>
       <c r="B36">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C36">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D36">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E36">
-        <v>0.19966220595159101</v>
+        <v>0.65688384913490006</v>
       </c>
       <c r="F36">
-        <v>0.19966220595159101</v>
+        <v>0.56162508846695203</v>
       </c>
       <c r="G36">
-        <v>0.19966220595159101</v>
+        <v>0.40593673391254598</v>
       </c>
       <c r="H36">
-        <v>0.19966220595159101</v>
+        <v>0.30993475094059397</v>
       </c>
       <c r="I36">
-        <v>1</v>
+        <v>1.87695196954741E-2</v>
       </c>
       <c r="J36">
-        <v>1</v>
+        <v>0.63488804766750195</v>
       </c>
       <c r="K36">
-        <v>1</v>
+        <v>-10</v>
       </c>
       <c r="L36" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M36" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="N36" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>2</v>
       </c>
       <c r="B37">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C37">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D37">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E37">
-        <v>8.4170453231757994E-2</v>
+        <v>0.27857501901371701</v>
       </c>
       <c r="F37">
-        <v>0.19966220595159101</v>
+        <v>0.56162508846695203</v>
       </c>
       <c r="G37">
-        <v>3.3342680140349398E-2</v>
+        <v>0.42216469549779001</v>
       </c>
       <c r="H37">
-        <v>0.19966220595159101</v>
+        <v>0.30993475094059397</v>
       </c>
       <c r="I37">
-        <v>-1.6735328751363301E-3</v>
+        <v>0.50057518439717696</v>
       </c>
       <c r="J37">
-        <v>1</v>
+        <v>0.63488804766750195</v>
       </c>
       <c r="K37">
-        <v>-10</v>
+        <v>0.28031055955788298</v>
       </c>
       <c r="L37" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M37" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="N37" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>2</v>
       </c>
       <c r="B38">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C38">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D38">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E38">
-        <v>0.566646675092223</v>
+        <v>0.31685573999791999</v>
       </c>
       <c r="F38">
-        <v>0.566646675092223</v>
+        <v>0.58470463432173803</v>
       </c>
       <c r="G38">
-        <v>0.566646675092223</v>
+        <v>0.56162508846695203</v>
       </c>
       <c r="H38">
-        <v>0.566646675092223</v>
+        <v>0.30993475094059397</v>
       </c>
       <c r="I38">
-        <v>1</v>
+        <v>0.76576267194731096</v>
       </c>
       <c r="J38">
-        <v>1</v>
+        <v>0.63488804766750195</v>
       </c>
       <c r="K38">
-        <v>1</v>
+        <v>-10</v>
       </c>
       <c r="L38" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M38" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N38" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>2</v>
+      </c>
+      <c r="B39">
+        <v>5</v>
+      </c>
+      <c r="C39">
+        <v>8</v>
+      </c>
+      <c r="D39">
+        <v>6</v>
+      </c>
+      <c r="E39">
+        <v>0.37215198973908198</v>
+      </c>
+      <c r="F39">
+        <v>0.56162508846695203</v>
+      </c>
+      <c r="G39">
+        <v>0.40593673391254598</v>
+      </c>
+      <c r="H39">
+        <v>0.30993475094059397</v>
+      </c>
+      <c r="I39">
+        <v>0.82429751941773199</v>
+      </c>
+      <c r="J39">
+        <v>0.63488804766750195</v>
+      </c>
+      <c r="K39">
+        <v>-10</v>
+      </c>
+      <c r="L39" t="s">
+        <v>21</v>
+      </c>
+      <c r="M39" t="s">
+        <v>27</v>
+      </c>
+      <c r="N39" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>2</v>
-      </c>
-      <c r="B39">
-        <v>4</v>
-      </c>
-      <c r="C39">
-        <v>4</v>
-      </c>
-      <c r="D39">
-        <v>4</v>
-      </c>
-      <c r="E39">
-        <v>0.566646675092223</v>
-      </c>
-      <c r="F39">
-        <v>0.566646675092223</v>
-      </c>
-      <c r="G39">
-        <v>0.566646675092223</v>
-      </c>
-      <c r="H39">
-        <v>0.566646675092223</v>
-      </c>
-      <c r="I39">
-        <v>1</v>
-      </c>
-      <c r="J39">
-        <v>1</v>
-      </c>
-      <c r="K39">
-        <v>1</v>
-      </c>
-      <c r="L39" t="s">
-        <v>22</v>
-      </c>
-      <c r="M39" t="s">
-        <v>25</v>
-      </c>
-      <c r="N39" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
@@ -2173,34 +2200,34 @@
         <v>4</v>
       </c>
       <c r="E40">
-        <v>0.566646675092223</v>
+        <v>0.49883257996769198</v>
       </c>
       <c r="F40">
-        <v>0.566646675092223</v>
+        <v>0.50354162084910403</v>
       </c>
       <c r="G40">
-        <v>0.566646675092223</v>
+        <v>0.50354162084910403</v>
       </c>
       <c r="H40">
-        <v>0.566646675092223</v>
+        <v>0.50354162084910403</v>
       </c>
       <c r="I40">
-        <v>1</v>
+        <v>0.98008594436669005</v>
       </c>
       <c r="J40">
         <v>1</v>
       </c>
       <c r="K40">
-        <v>1</v>
+        <v>0.98008594436669005</v>
       </c>
       <c r="L40" t="s">
         <v>22</v>
       </c>
       <c r="M40" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="N40" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
@@ -2208,7 +2235,7 @@
         <v>2</v>
       </c>
       <c r="B41">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C41">
         <v>4</v>
@@ -2217,34 +2244,34 @@
         <v>4</v>
       </c>
       <c r="E41">
-        <v>0.566646675092223</v>
+        <v>0.29309016613321198</v>
       </c>
       <c r="F41">
-        <v>0.566646675092223</v>
+        <v>0.50354162084910403</v>
       </c>
       <c r="G41">
-        <v>0.566646675092223</v>
+        <v>0.28473904387460602</v>
       </c>
       <c r="H41">
-        <v>0.566646675092223</v>
+        <v>0.50354162084910403</v>
       </c>
       <c r="I41">
-        <v>1</v>
+        <v>0.17879836972409099</v>
       </c>
       <c r="J41">
         <v>1</v>
       </c>
       <c r="K41">
-        <v>1</v>
+        <v>-10</v>
       </c>
       <c r="L41" t="s">
         <v>22</v>
       </c>
       <c r="M41" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="N41" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
@@ -2252,25 +2279,25 @@
         <v>2</v>
       </c>
       <c r="B42">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C42">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D42">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E42">
-        <v>0.48591870935773301</v>
+        <v>0.19966220595159101</v>
       </c>
       <c r="F42">
-        <v>0.48591870935773301</v>
+        <v>0.19966220595159101</v>
       </c>
       <c r="G42">
-        <v>0.48591870935773301</v>
+        <v>0.19966220595159101</v>
       </c>
       <c r="H42">
-        <v>0.48591870935773301</v>
+        <v>0.19966220595159101</v>
       </c>
       <c r="I42">
         <v>1</v>
@@ -2282,10 +2309,10 @@
         <v>1</v>
       </c>
       <c r="L42" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M42" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="N42" t="s">
         <v>16</v>
@@ -2299,301 +2326,301 @@
         <v>2</v>
       </c>
       <c r="C43">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D43">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E43">
-        <v>0.48591870935773301</v>
+        <v>8.4170453231757994E-2</v>
       </c>
       <c r="F43">
-        <v>0.48591870935773301</v>
+        <v>0.19966220595159101</v>
       </c>
       <c r="G43">
-        <v>0.48591870935773301</v>
+        <v>3.3342680140349398E-2</v>
       </c>
       <c r="H43">
-        <v>0.48591870935773301</v>
+        <v>0.19966220595159101</v>
       </c>
       <c r="I43">
-        <v>1</v>
+        <v>-1.6735328751363301E-3</v>
       </c>
       <c r="J43">
         <v>1</v>
       </c>
       <c r="K43">
-        <v>1</v>
+        <v>-10</v>
       </c>
       <c r="L43" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M43" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="N43" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>2</v>
       </c>
       <c r="B44">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C44">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D44">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E44">
-        <v>4.3543955614666202E-2</v>
+        <v>0.566646675092223</v>
       </c>
       <c r="F44">
-        <v>2.2004889975551899E-2</v>
+        <v>0.566646675092223</v>
       </c>
       <c r="G44">
-        <v>2.2004889975551899E-2</v>
+        <v>0.566646675092223</v>
       </c>
       <c r="H44">
-        <v>2.2004889975551899E-2</v>
+        <v>0.566646675092223</v>
       </c>
       <c r="I44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J44">
         <v>1</v>
       </c>
       <c r="K44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L44" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M44" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="N44" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>2</v>
+      </c>
+      <c r="B45">
+        <v>4</v>
+      </c>
+      <c r="C45">
+        <v>4</v>
+      </c>
+      <c r="D45">
+        <v>4</v>
+      </c>
+      <c r="E45">
+        <v>0.566646675092223</v>
+      </c>
+      <c r="F45">
+        <v>0.566646675092223</v>
+      </c>
+      <c r="G45">
+        <v>0.566646675092223</v>
+      </c>
+      <c r="H45">
+        <v>0.566646675092223</v>
+      </c>
+      <c r="I45">
+        <v>1</v>
+      </c>
+      <c r="J45">
+        <v>1</v>
+      </c>
+      <c r="K45">
+        <v>1</v>
+      </c>
+      <c r="L45" t="s">
+        <v>22</v>
+      </c>
+      <c r="M45" t="s">
+        <v>25</v>
+      </c>
+      <c r="N45" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <v>2</v>
-      </c>
-      <c r="B45">
-        <v>2</v>
-      </c>
-      <c r="C45">
-        <v>2</v>
-      </c>
-      <c r="D45">
-        <v>2</v>
-      </c>
-      <c r="E45">
-        <v>4.3543955614666202E-2</v>
-      </c>
-      <c r="F45">
-        <v>2.2004889975551899E-2</v>
-      </c>
-      <c r="G45">
-        <v>2.2004889975551899E-2</v>
-      </c>
-      <c r="H45">
-        <v>2.2004889975551899E-2</v>
-      </c>
-      <c r="I45">
-        <v>0</v>
-      </c>
-      <c r="J45">
-        <v>1</v>
-      </c>
-      <c r="K45">
-        <v>0</v>
-      </c>
-      <c r="L45" t="s">
-        <v>23</v>
-      </c>
-      <c r="M45" t="s">
-        <v>18</v>
-      </c>
-      <c r="N45" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>2</v>
       </c>
       <c r="B46">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C46">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D46">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E46">
-        <v>9.4521336230725103E-2</v>
+        <v>0.566646675092223</v>
       </c>
       <c r="F46">
-        <v>0.30348431620673499</v>
+        <v>0.566646675092223</v>
       </c>
       <c r="G46">
-        <v>0.30348431620673499</v>
+        <v>0.566646675092223</v>
       </c>
       <c r="H46">
-        <v>0.30348431620673499</v>
+        <v>0.566646675092223</v>
       </c>
       <c r="I46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J46">
         <v>1</v>
       </c>
       <c r="K46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L46" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M46" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N46" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>2</v>
       </c>
       <c r="B47">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C47">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D47">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E47">
-        <v>0.21130577583669299</v>
+        <v>0.566646675092223</v>
       </c>
       <c r="F47">
-        <v>0.30348431620673499</v>
+        <v>0.566646675092223</v>
       </c>
       <c r="G47">
-        <v>0.23507367651524499</v>
+        <v>0.566646675092223</v>
       </c>
       <c r="H47">
-        <v>0.30348431620673499</v>
+        <v>0.566646675092223</v>
       </c>
       <c r="I47">
-        <v>0.31467534132427399</v>
+        <v>1</v>
       </c>
       <c r="J47">
         <v>1</v>
       </c>
       <c r="K47">
-        <v>-10</v>
+        <v>1</v>
       </c>
       <c r="L47" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M47" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N47" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>2</v>
       </c>
       <c r="B48">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C48">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D48">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E48">
-        <v>0.28677139046572198</v>
+        <v>0.566646675092223</v>
       </c>
       <c r="F48">
-        <v>0.30348431620673499</v>
+        <v>0.566646675092223</v>
       </c>
       <c r="G48">
-        <v>0.29197914425018001</v>
+        <v>0.566646675092223</v>
       </c>
       <c r="H48">
-        <v>0.30348431620673499</v>
+        <v>0.566646675092223</v>
       </c>
       <c r="I48">
-        <v>0.37777987991544798</v>
+        <v>1</v>
       </c>
       <c r="J48">
         <v>1</v>
       </c>
       <c r="K48">
-        <v>-10</v>
+        <v>1</v>
       </c>
       <c r="L48" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M48" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N48" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>2</v>
       </c>
       <c r="B49">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C49">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D49">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E49">
-        <v>0.28677139046572198</v>
+        <v>0.566646675092223</v>
       </c>
       <c r="F49">
-        <v>0.30348431620673499</v>
+        <v>0.566646675092223</v>
       </c>
       <c r="G49">
-        <v>0.29197914425018001</v>
+        <v>0.566646675092223</v>
       </c>
       <c r="H49">
-        <v>0.30348431620673499</v>
+        <v>0.566646675092223</v>
       </c>
       <c r="I49">
-        <v>0.37777987991544798</v>
+        <v>1</v>
       </c>
       <c r="J49">
         <v>1</v>
       </c>
       <c r="K49">
-        <v>-10</v>
+        <v>1</v>
       </c>
       <c r="L49" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M49" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N49" t="s">
         <v>16</v>
@@ -2607,34 +2634,34 @@
         <v>2</v>
       </c>
       <c r="C50">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D50">
         <v>2</v>
       </c>
       <c r="E50">
-        <v>0.40647553623541899</v>
+        <v>0.48591870935773301</v>
       </c>
       <c r="F50">
-        <v>0.42326937558428301</v>
+        <v>0.48591870935773301</v>
       </c>
       <c r="G50">
-        <v>0.40850268959332903</v>
+        <v>0.48591870935773301</v>
       </c>
       <c r="H50">
-        <v>0.383884919047985</v>
+        <v>0.48591870935773301</v>
       </c>
       <c r="I50">
-        <v>0.20779325299204801</v>
+        <v>1</v>
       </c>
       <c r="J50">
-        <v>0.85584718950503003</v>
+        <v>1</v>
       </c>
       <c r="K50">
-        <v>0.14500318826151101</v>
+        <v>1</v>
       </c>
       <c r="L50" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M50" t="s">
         <v>15</v>
@@ -2651,34 +2678,34 @@
         <v>2</v>
       </c>
       <c r="C51">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D51">
         <v>2</v>
       </c>
       <c r="E51">
-        <v>0.383884919047985</v>
+        <v>0.48591870935773301</v>
       </c>
       <c r="F51">
-        <v>0.42326937558428301</v>
+        <v>0.48591870935773301</v>
       </c>
       <c r="G51">
-        <v>0.40850268959332903</v>
+        <v>0.48591870935773301</v>
       </c>
       <c r="H51">
-        <v>0.383884919047985</v>
+        <v>0.48591870935773301</v>
       </c>
       <c r="I51">
-        <v>0.85584718950503003</v>
+        <v>1</v>
       </c>
       <c r="J51">
-        <v>0.85584718950503003</v>
+        <v>1</v>
       </c>
       <c r="K51">
         <v>1</v>
       </c>
       <c r="L51" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M51" t="s">
         <v>15</v>
@@ -2695,34 +2722,34 @@
         <v>2</v>
       </c>
       <c r="C52">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D52">
         <v>2</v>
       </c>
       <c r="E52">
-        <v>6.3259612457336106E-2</v>
+        <v>4.3543955614666202E-2</v>
       </c>
       <c r="F52">
-        <v>2.37448582176614E-2</v>
+        <v>2.2004889975551899E-2</v>
       </c>
       <c r="G52">
-        <v>1.9132304679876099E-2</v>
+        <v>2.2004889975551899E-2</v>
       </c>
       <c r="H52">
-        <v>6.3259612457336106E-2</v>
+        <v>2.2004889975551899E-2</v>
       </c>
       <c r="I52">
-        <v>0.85584718950503003</v>
+        <v>0</v>
       </c>
       <c r="J52">
-        <v>0.85584718950503003</v>
+        <v>1</v>
       </c>
       <c r="K52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L52" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M52" t="s">
         <v>18</v>
@@ -2739,34 +2766,34 @@
         <v>2</v>
       </c>
       <c r="C53">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D53">
         <v>2</v>
       </c>
       <c r="E53">
-        <v>6.3259612457336106E-2</v>
+        <v>4.3543955614666202E-2</v>
       </c>
       <c r="F53">
-        <v>2.37448582176614E-2</v>
+        <v>2.2004889975551899E-2</v>
       </c>
       <c r="G53">
-        <v>1.9132304679876099E-2</v>
+        <v>2.2004889975551899E-2</v>
       </c>
       <c r="H53">
-        <v>6.3259612457336106E-2</v>
+        <v>2.2004889975551899E-2</v>
       </c>
       <c r="I53">
-        <v>0.85584718950503003</v>
+        <v>0</v>
       </c>
       <c r="J53">
-        <v>0.85584718950503003</v>
+        <v>1</v>
       </c>
       <c r="K53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L53" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M53" t="s">
         <v>18</v>
@@ -2775,7 +2802,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>2</v>
       </c>
@@ -2783,34 +2810,34 @@
         <v>2</v>
       </c>
       <c r="C54">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D54">
         <v>2</v>
       </c>
       <c r="E54">
-        <v>0.19581557688418499</v>
+        <v>9.4521336230725103E-2</v>
       </c>
       <c r="F54">
-        <v>0.29482035565072501</v>
+        <v>0.30348431620673499</v>
       </c>
       <c r="G54">
-        <v>0.21210964210571401</v>
+        <v>0.30348431620673499</v>
       </c>
       <c r="H54">
-        <v>0.19581557688418499</v>
+        <v>0.30348431620673499</v>
       </c>
       <c r="I54">
-        <v>0.85584718950503003</v>
+        <v>0</v>
       </c>
       <c r="J54">
-        <v>0.85584718950503003</v>
+        <v>1</v>
       </c>
       <c r="K54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M54" t="s">
         <v>25</v>
@@ -2819,42 +2846,42 @@
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>2</v>
       </c>
       <c r="B55">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C55">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D55">
         <v>2</v>
       </c>
       <c r="E55">
-        <v>0.192562401498757</v>
+        <v>0.21130577583669299</v>
       </c>
       <c r="F55">
-        <v>0.29482035565072501</v>
+        <v>0.30348431620673499</v>
       </c>
       <c r="G55">
-        <v>0.238230082161111</v>
+        <v>0.23507367651524499</v>
       </c>
       <c r="H55">
-        <v>0.19581557688418499</v>
+        <v>0.30348431620673499</v>
       </c>
       <c r="I55">
-        <v>0.39940445212331999</v>
+        <v>0.31467534132427399</v>
       </c>
       <c r="J55">
-        <v>0.85584718950503003</v>
+        <v>1</v>
       </c>
       <c r="K55">
         <v>-10</v>
       </c>
       <c r="L55" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M55" t="s">
         <v>25</v>
@@ -2863,42 +2890,42 @@
         <v>16</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>2</v>
       </c>
       <c r="B56">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C56">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D56">
         <v>2</v>
       </c>
       <c r="E56">
-        <v>0.19581557688418499</v>
+        <v>0.28677139046572198</v>
       </c>
       <c r="F56">
-        <v>0.29482035565072501</v>
+        <v>0.30348431620673499</v>
       </c>
       <c r="G56">
-        <v>0.21210964210571401</v>
+        <v>0.29197914425018001</v>
       </c>
       <c r="H56">
-        <v>0.19581557688418499</v>
+        <v>0.30348431620673499</v>
       </c>
       <c r="I56">
-        <v>0.85584718950503003</v>
+        <v>0.37777987991544798</v>
       </c>
       <c r="J56">
-        <v>0.85584718950503003</v>
+        <v>1</v>
       </c>
       <c r="K56">
-        <v>1</v>
+        <v>-10</v>
       </c>
       <c r="L56" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M56" t="s">
         <v>26</v>
@@ -2907,42 +2934,42 @@
         <v>17</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>2</v>
       </c>
       <c r="B57">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C57">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D57">
         <v>2</v>
       </c>
       <c r="E57">
-        <v>0.19581557688418499</v>
+        <v>0.28677139046572198</v>
       </c>
       <c r="F57">
-        <v>0.29482035565072501</v>
+        <v>0.30348431620673499</v>
       </c>
       <c r="G57">
-        <v>0.21210964210571401</v>
+        <v>0.29197914425018001</v>
       </c>
       <c r="H57">
-        <v>0.19581557688418499</v>
+        <v>0.30348431620673499</v>
       </c>
       <c r="I57">
-        <v>0.85584718950503003</v>
+        <v>0.37777987991544798</v>
       </c>
       <c r="J57">
-        <v>0.85584718950503003</v>
+        <v>1</v>
       </c>
       <c r="K57">
-        <v>1</v>
+        <v>-10</v>
       </c>
       <c r="L57" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M57" t="s">
         <v>26</v>
@@ -2951,10 +2978,500 @@
         <v>16</v>
       </c>
     </row>
+    <row r="58" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>2</v>
+      </c>
+      <c r="B58">
+        <v>2</v>
+      </c>
+      <c r="C58">
+        <v>2</v>
+      </c>
+      <c r="D58">
+        <v>2</v>
+      </c>
+      <c r="E58">
+        <v>0.30348431620673499</v>
+      </c>
+      <c r="F58">
+        <v>0.30348431620673499</v>
+      </c>
+      <c r="G58">
+        <v>0.30348431620673499</v>
+      </c>
+      <c r="H58">
+        <v>0.30348431620673499</v>
+      </c>
+      <c r="I58">
+        <v>1</v>
+      </c>
+      <c r="J58">
+        <v>1</v>
+      </c>
+      <c r="K58">
+        <v>1</v>
+      </c>
+      <c r="L58" t="s">
+        <v>23</v>
+      </c>
+      <c r="M58" t="s">
+        <v>27</v>
+      </c>
+      <c r="N58" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>2</v>
+      </c>
+      <c r="B59">
+        <v>6</v>
+      </c>
+      <c r="C59">
+        <v>2</v>
+      </c>
+      <c r="D59">
+        <v>2</v>
+      </c>
+      <c r="E59">
+        <v>0.31218291692039102</v>
+      </c>
+      <c r="F59">
+        <v>0.30348431620673499</v>
+      </c>
+      <c r="G59">
+        <v>0.223228447380481</v>
+      </c>
+      <c r="H59">
+        <v>0.30348431620673499</v>
+      </c>
+      <c r="I59">
+        <v>0.43836334277738298</v>
+      </c>
+      <c r="J59">
+        <v>1</v>
+      </c>
+      <c r="K59">
+        <v>-10</v>
+      </c>
+      <c r="L59" t="s">
+        <v>23</v>
+      </c>
+      <c r="M59" t="s">
+        <v>27</v>
+      </c>
+      <c r="N59" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>2</v>
+      </c>
+      <c r="B60">
+        <v>2</v>
+      </c>
+      <c r="C60">
+        <v>4</v>
+      </c>
+      <c r="D60">
+        <v>2</v>
+      </c>
+      <c r="E60">
+        <v>0.40647553623541899</v>
+      </c>
+      <c r="F60">
+        <v>0.42326937558428301</v>
+      </c>
+      <c r="G60">
+        <v>0.40850268959332903</v>
+      </c>
+      <c r="H60">
+        <v>0.383884919047985</v>
+      </c>
+      <c r="I60">
+        <v>0.20779325299204801</v>
+      </c>
+      <c r="J60">
+        <v>0.85584718950503003</v>
+      </c>
+      <c r="K60">
+        <v>0.14500318826151101</v>
+      </c>
+      <c r="L60" t="s">
+        <v>24</v>
+      </c>
+      <c r="M60" t="s">
+        <v>15</v>
+      </c>
+      <c r="N60" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>2</v>
+      </c>
+      <c r="B61">
+        <v>2</v>
+      </c>
+      <c r="C61">
+        <v>4</v>
+      </c>
+      <c r="D61">
+        <v>2</v>
+      </c>
+      <c r="E61">
+        <v>0.383884919047985</v>
+      </c>
+      <c r="F61">
+        <v>0.42326937558428301</v>
+      </c>
+      <c r="G61">
+        <v>0.40850268959332903</v>
+      </c>
+      <c r="H61">
+        <v>0.383884919047985</v>
+      </c>
+      <c r="I61">
+        <v>0.85584718950503003</v>
+      </c>
+      <c r="J61">
+        <v>0.85584718950503003</v>
+      </c>
+      <c r="K61">
+        <v>1</v>
+      </c>
+      <c r="L61" t="s">
+        <v>24</v>
+      </c>
+      <c r="M61" t="s">
+        <v>15</v>
+      </c>
+      <c r="N61" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>2</v>
+      </c>
+      <c r="B62">
+        <v>2</v>
+      </c>
+      <c r="C62">
+        <v>4</v>
+      </c>
+      <c r="D62">
+        <v>2</v>
+      </c>
+      <c r="E62">
+        <v>6.3259612457336106E-2</v>
+      </c>
+      <c r="F62">
+        <v>2.37448582176614E-2</v>
+      </c>
+      <c r="G62">
+        <v>1.9132304679876099E-2</v>
+      </c>
+      <c r="H62">
+        <v>6.3259612457336106E-2</v>
+      </c>
+      <c r="I62">
+        <v>0.85584718950503003</v>
+      </c>
+      <c r="J62">
+        <v>0.85584718950503003</v>
+      </c>
+      <c r="K62">
+        <v>1</v>
+      </c>
+      <c r="L62" t="s">
+        <v>24</v>
+      </c>
+      <c r="M62" t="s">
+        <v>18</v>
+      </c>
+      <c r="N62" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>2</v>
+      </c>
+      <c r="B63">
+        <v>2</v>
+      </c>
+      <c r="C63">
+        <v>4</v>
+      </c>
+      <c r="D63">
+        <v>2</v>
+      </c>
+      <c r="E63">
+        <v>6.3259612457336106E-2</v>
+      </c>
+      <c r="F63">
+        <v>2.37448582176614E-2</v>
+      </c>
+      <c r="G63">
+        <v>1.9132304679876099E-2</v>
+      </c>
+      <c r="H63">
+        <v>6.3259612457336106E-2</v>
+      </c>
+      <c r="I63">
+        <v>0.85584718950503003</v>
+      </c>
+      <c r="J63">
+        <v>0.85584718950503003</v>
+      </c>
+      <c r="K63">
+        <v>1</v>
+      </c>
+      <c r="L63" t="s">
+        <v>24</v>
+      </c>
+      <c r="M63" t="s">
+        <v>18</v>
+      </c>
+      <c r="N63" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>2</v>
+      </c>
+      <c r="B64">
+        <v>2</v>
+      </c>
+      <c r="C64">
+        <v>4</v>
+      </c>
+      <c r="D64">
+        <v>2</v>
+      </c>
+      <c r="E64">
+        <v>0.19581557688418499</v>
+      </c>
+      <c r="F64">
+        <v>0.29482035565072501</v>
+      </c>
+      <c r="G64">
+        <v>0.21210964210571401</v>
+      </c>
+      <c r="H64">
+        <v>0.19581557688418499</v>
+      </c>
+      <c r="I64">
+        <v>0.85584718950503003</v>
+      </c>
+      <c r="J64">
+        <v>0.85584718950503003</v>
+      </c>
+      <c r="K64">
+        <v>1</v>
+      </c>
+      <c r="L64" t="s">
+        <v>24</v>
+      </c>
+      <c r="M64" t="s">
+        <v>25</v>
+      </c>
+      <c r="N64" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>2</v>
+      </c>
+      <c r="B65">
+        <v>5</v>
+      </c>
+      <c r="C65">
+        <v>4</v>
+      </c>
+      <c r="D65">
+        <v>2</v>
+      </c>
+      <c r="E65">
+        <v>0.192562401498757</v>
+      </c>
+      <c r="F65">
+        <v>0.29482035565072501</v>
+      </c>
+      <c r="G65">
+        <v>0.238230082161111</v>
+      </c>
+      <c r="H65">
+        <v>0.19581557688418499</v>
+      </c>
+      <c r="I65">
+        <v>0.39940445212331999</v>
+      </c>
+      <c r="J65">
+        <v>0.85584718950503003</v>
+      </c>
+      <c r="K65">
+        <v>-10</v>
+      </c>
+      <c r="L65" t="s">
+        <v>24</v>
+      </c>
+      <c r="M65" t="s">
+        <v>25</v>
+      </c>
+      <c r="N65" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>2</v>
+      </c>
+      <c r="B66">
+        <v>2</v>
+      </c>
+      <c r="C66">
+        <v>4</v>
+      </c>
+      <c r="D66">
+        <v>2</v>
+      </c>
+      <c r="E66">
+        <v>0.19581557688418499</v>
+      </c>
+      <c r="F66">
+        <v>0.29482035565072501</v>
+      </c>
+      <c r="G66">
+        <v>0.21210964210571401</v>
+      </c>
+      <c r="H66">
+        <v>0.19581557688418499</v>
+      </c>
+      <c r="I66">
+        <v>0.85584718950503003</v>
+      </c>
+      <c r="J66">
+        <v>0.85584718950503003</v>
+      </c>
+      <c r="K66">
+        <v>1</v>
+      </c>
+      <c r="L66" t="s">
+        <v>24</v>
+      </c>
+      <c r="M66" t="s">
+        <v>26</v>
+      </c>
+      <c r="N66" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>2</v>
+      </c>
+      <c r="B67">
+        <v>2</v>
+      </c>
+      <c r="C67">
+        <v>4</v>
+      </c>
+      <c r="D67">
+        <v>2</v>
+      </c>
+      <c r="E67">
+        <v>0.19581557688418499</v>
+      </c>
+      <c r="F67">
+        <v>0.29482035565072501</v>
+      </c>
+      <c r="G67">
+        <v>0.21210964210571401</v>
+      </c>
+      <c r="H67">
+        <v>0.19581557688418499</v>
+      </c>
+      <c r="I67">
+        <v>0.85584718950503003</v>
+      </c>
+      <c r="J67">
+        <v>0.85584718950503003</v>
+      </c>
+      <c r="K67">
+        <v>1</v>
+      </c>
+      <c r="L67" t="s">
+        <v>24</v>
+      </c>
+      <c r="M67" t="s">
+        <v>26</v>
+      </c>
+      <c r="N67" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>2</v>
+      </c>
+      <c r="B68">
+        <v>4</v>
+      </c>
+      <c r="C68">
+        <v>4</v>
+      </c>
+      <c r="D68">
+        <v>2</v>
+      </c>
+      <c r="E68">
+        <v>0.24796840255685501</v>
+      </c>
+      <c r="F68">
+        <v>0.29482035565072501</v>
+      </c>
+      <c r="G68">
+        <v>0.29482035565072501</v>
+      </c>
+      <c r="H68">
+        <v>0.19581557688418499</v>
+      </c>
+      <c r="I68">
+        <v>0.56990648688255696</v>
+      </c>
+      <c r="J68">
+        <v>0.85584718950503003</v>
+      </c>
+      <c r="K68">
+        <v>-10</v>
+      </c>
+      <c r="L68" t="s">
+        <v>24</v>
+      </c>
+      <c r="M68" t="s">
+        <v>27</v>
+      </c>
+      <c r="N68" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:N57">
-    <sortState ref="A2:N57">
-      <sortCondition ref="L1:L57"/>
+  <autoFilter ref="A1:N68">
+    <filterColumn colId="12">
+      <filters>
+        <filter val="dunnindex"/>
+        <filter val="silhouette"/>
+      </filters>
+    </filterColumn>
+    <sortState ref="A2:N68">
+      <sortCondition ref="L1:L68"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>